<commit_message>
A-2 Building mains reports
</commit_message>
<xml_diff>
--- a/support_data/outloads/dict_nom.xlsx
+++ b/support_data/outloads/dict_nom.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20354"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF91461-1620-4D9E-A7FF-5606265422F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA324F0E-8EDB-4256-ADC0-471A54F03BB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17677" uniqueCount="3741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17687" uniqueCount="3743">
   <si>
     <t>Номенклатура</t>
   </si>
@@ -11241,6 +11241,12 @@
   </si>
   <si>
     <t>нд</t>
+  </si>
+  <si>
+    <t>Круг 110 ГОСТ 2590-2006 ст3 ГОСТ 380-2005</t>
+  </si>
+  <si>
+    <t>Труба 127х10 ГОСТ 8732-78 ст3 ГОСТ 380-2005</t>
   </si>
 </sst>
 </file>
@@ -11628,10 +11634,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:F3051"/>
+  <dimension ref="A1:F3053"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3002" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3051" sqref="F3051"/>
+    <sheetView tabSelected="1" topLeftCell="A3016" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3052" sqref="A3052"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72663,6 +72669,46 @@
         <v>3740</v>
       </c>
     </row>
+    <row r="3052" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3052" t="s">
+        <v>3741</v>
+      </c>
+      <c r="B3052" t="s">
+        <v>3476</v>
+      </c>
+      <c r="C3052" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3052" t="s">
+        <v>3086</v>
+      </c>
+      <c r="E3052">
+        <v>0</v>
+      </c>
+      <c r="F3052" t="s">
+        <v>3087</v>
+      </c>
+    </row>
+    <row r="3053" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3053" t="s">
+        <v>3742</v>
+      </c>
+      <c r="B3053" t="s">
+        <v>3297</v>
+      </c>
+      <c r="C3053" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3053" t="s">
+        <v>3086</v>
+      </c>
+      <c r="E3053">
+        <v>0</v>
+      </c>
+      <c r="F3053" t="s">
+        <v>3087</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F1563" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="A2:A842">

</xml_diff>